<commit_message>
Fixed invalid test file contents (not format-related) and fixed AnimalLoadingTests.
This file:

- DataRepo/example_data/testing_data/animal_sample_table_labeled_elements.xlsx

contained elements not present in the compound on the row (I think it was valine).  I replaced it with methionine, which happens to have all currently supported elements.

Files checked in: DataRepo/example_data/testing_data/animal_sample_table_labeled_elements.xlsx DataRepo/tests/test_models.py
[skip ci]
</commit_message>
<xml_diff>
--- a/DataRepo/example_data/testing_data/animal_sample_table_labeled_elements.xlsx
+++ b/DataRepo/example_data/testing_data/animal_sample_table_labeled_elements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-local/TRACEBASE/tracebase/DataRepo/example_data/testing_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-LOCAL/TRACEBASE/tracebase/DataRepo/example_data/testing_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2561384D-7365-3242-9954-82CF45337991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7C6D405C-90A7-0044-8E4B-6BBCBB496537}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24640" windowHeight="9980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24640" windowHeight="9980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Animals" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Treatments" sheetId="3" r:id="rId3"/>
     <sheet name="Tissues" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="102">
   <si>
     <t>Animal ID</t>
   </si>
@@ -96,9 +96,6 @@
     <t>test_animal_5</t>
   </si>
   <si>
-    <t>test_animal_6</t>
-  </si>
-  <si>
     <t>Sample Name</t>
   </si>
   <si>
@@ -138,9 +135,6 @@
     <t>test_animal_5_sample_1</t>
   </si>
   <si>
-    <t>test_animal_6_sample_1</t>
-  </si>
-  <si>
     <t>Treatment Description</t>
   </si>
   <si>
@@ -324,22 +318,22 @@
     <t>Infusate</t>
   </si>
   <si>
-    <t>glucose-[13C6]</t>
-  </si>
-  <si>
-    <t>glucose-[15N6]</t>
-  </si>
-  <si>
-    <t>glucose-[2H6]</t>
-  </si>
-  <si>
-    <t>glucose-[17O6]</t>
-  </si>
-  <si>
-    <t>glucose-[33S6]</t>
-  </si>
-  <si>
     <t>Tracer Concentrations</t>
+  </si>
+  <si>
+    <t>methionine-[13C5]</t>
+  </si>
+  <si>
+    <t>methionine-[15N1]</t>
+  </si>
+  <si>
+    <t>methionine-[2H11]</t>
+  </si>
+  <si>
+    <t>methionine-[17O2]</t>
+  </si>
+  <si>
+    <t>methionine-[33S1]</t>
   </si>
 </sst>
 </file>
@@ -706,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -718,7 +712,7 @@
     <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
     <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
@@ -742,13 +736,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -780,7 +774,7 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F2">
         <v>0.1</v>
@@ -815,7 +809,7 @@
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F3">
         <v>0.1</v>
@@ -850,7 +844,7 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F4">
         <v>0.1</v>
@@ -885,7 +879,7 @@
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F5">
         <v>0.1</v>
@@ -920,7 +914,7 @@
         <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F6">
         <v>0.1</v>
@@ -938,41 +932,6 @@
         <v>15</v>
       </c>
       <c r="K6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F7">
-        <v>0.1</v>
-      </c>
-      <c r="G7">
-        <v>200</v>
-      </c>
-      <c r="H7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -984,29 +943,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
@@ -1014,19 +981,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2">
         <v>44537</v>
       </c>
       <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>31</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -1034,19 +1001,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2">
         <v>44537</v>
       </c>
       <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
         <v>29</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>31</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -1054,19 +1021,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2">
         <v>44537</v>
       </c>
       <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
         <v>29</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>30</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
       </c>
       <c r="F4" t="s">
         <v>19</v>
@@ -1074,19 +1041,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2">
         <v>44537</v>
       </c>
       <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
         <v>29</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>30</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
@@ -1094,42 +1061,22 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2">
         <v>44537</v>
       </c>
       <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>30</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
       </c>
       <c r="F6" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="2">
-        <v>44537</v>
-      </c>
-      <c r="C7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1142,16 +1089,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="130.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1159,7 +1112,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1172,296 +1125,302 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B32" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B33" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B34" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>